<commit_message>
Últimas actualizaciones documentación, prueba inicial corregir error en funcionalidad de contraseña olvidada.
</commit_message>
<xml_diff>
--- a/Documentación/Resultados/Resultados.xlsx
+++ b/Documentación/Resultados/Resultados.xlsx
@@ -8,45 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Universidad\Máster\Segundo_semestre\Planificación y Gestión de Infraestructuras TIC\Practicas\ABP\Proyecto-PYGITIC-2020\Documentación\Resultados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE268DD7-95AD-4E29-8E2F-416C8B64BD07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0F828BE-7B97-4A52-98BB-D4814F6E5687}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Hoja1!$I$10:$U$10</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Hoja1!$I$11:$U$11</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Hoja1!$I$11:$U$11</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Hoja1!$I$3:$U$3</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Hoja1!$I$4:$U$4</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Hoja1!$I$5:$U$5</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">Hoja1!$I$6:$U$6</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">Hoja1!$I$7:$U$7</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">Hoja1!$I$8:$U$8</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">Hoja1!$I$9:$U$9</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">Hoja1!$I$10:$U$10</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">Hoja1!$I$11:$U$11</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Hoja1!$I$3:$U$3</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">Hoja1!$I$3:$U$3</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">Hoja1!$I$4:$U$4</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">Hoja1!$I$5:$U$5</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">Hoja1!$I$6:$U$6</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">Hoja1!$I$7:$U$7</definedName>
-    <definedName name="_xlchart.v1.25" hidden="1">Hoja1!$I$8:$U$8</definedName>
-    <definedName name="_xlchart.v1.26" hidden="1">Hoja1!$I$9:$U$9</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Hoja1!$I$4:$U$4</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Hoja1!$I$5:$U$5</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Hoja1!$I$6:$U$6</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Hoja1!$I$7:$U$7</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Hoja1!$I$8:$U$8</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Hoja1!$I$9:$U$9</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Hoja1!$I$10:$U$10</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -65,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="40">
   <si>
     <t>createdAt (S)</t>
   </si>
@@ -176,6 +144,15 @@
   </si>
   <si>
     <t>°C</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Enfermos</t>
+  </si>
+  <si>
+    <t>Sanos</t>
   </si>
 </sst>
 </file>
@@ -183,7 +160,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -359,13 +336,13 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -376,12 +353,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bueno" xfId="1" builtinId="26"/>
@@ -389,15 +369,7 @@
     <cellStyle name="Incorrecto" xfId="2" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF4B4B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -413,19 +385,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="cognitoLogs"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -691,10 +650,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:AA42"/>
+  <dimension ref="A2:AD42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="AE17" sqref="AE17"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="AC3" sqref="AC3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -712,7 +671,7 @@
     <col min="27" max="27" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -735,7 +694,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -796,8 +755,11 @@
       <c r="AA3" s="8" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AC3" s="16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -864,8 +826,14 @@
       <c r="AA4" s="11" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AC4" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -917,8 +885,16 @@
       <c r="AA5" s="14" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AC5">
+        <f>COUNTIF(AA4:AA21,TRUE)</f>
+        <v>11</v>
+      </c>
+      <c r="AD5">
+        <f>COUNTIF(AA5:AA22,FALSE)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -971,7 +947,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1016,7 +992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -1061,7 +1037,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -1106,7 +1082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -1151,7 +1127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -1196,7 +1172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
@@ -1237,7 +1213,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -1278,7 +1254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
@@ -1319,7 +1295,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -1360,7 +1336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
Arreglando excel con tabla resultados, una operación no contaba un caso.
</commit_message>
<xml_diff>
--- a/Documentación/Resultados/Resultados.xlsx
+++ b/Documentación/Resultados/Resultados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Universidad\Máster\Segundo_semestre\Planificación y Gestión de Infraestructuras TIC\Practicas\ABP\Proyecto-PYGITIC-2020\Documentación\Resultados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0F828BE-7B97-4A52-98BB-D4814F6E5687}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2FBF57F-95DE-4584-994D-D0A9B2D78AC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -653,7 +653,7 @@
   <dimension ref="A2:AD42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="AC3" sqref="AC3"/>
+      <selection activeCell="AC14" sqref="AC14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -890,8 +890,8 @@
         <v>11</v>
       </c>
       <c r="AD5">
-        <f>COUNTIF(AA5:AA22,FALSE)</f>
-        <v>6</v>
+        <f>COUNTIF(AA4:AA21,FALSE)</f>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">

</xml_diff>